<commit_message>
Rerun collection of codon_groups.xlsx
</commit_message>
<xml_diff>
--- a/Published/Figure_4/Main/Data/codon_groups.xlsx
+++ b/Published/Figure_4/Main/Data/codon_groups.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t xml:space="preserve">frequently_used</t>
   </si>
@@ -126,13 +126,13 @@
     <t xml:space="preserve">TGG</t>
   </si>
   <si>
-    <t xml:space="preserve">TAG</t>
+    <t xml:space="preserve">TCA</t>
   </si>
   <si>
     <t xml:space="preserve">CTG</t>
   </si>
   <si>
-    <t xml:space="preserve">TCA</t>
+    <t xml:space="preserve">TTA</t>
   </si>
   <si>
     <t xml:space="preserve">GAG</t>
@@ -144,9 +144,6 @@
     <t xml:space="preserve">CGT</t>
   </si>
   <si>
-    <t xml:space="preserve">TTA</t>
-  </si>
-  <si>
     <t xml:space="preserve">TTG</t>
   </si>
   <si>
@@ -163,12 +160,6 @@
   </si>
   <si>
     <t xml:space="preserve">ATC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGA</t>
   </si>
   <si>
     <t xml:space="preserve">ACG</t>
@@ -180,7 +171,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -499,10 +490,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -773,62 +764,40 @@
       <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15"/>
+      <c r="D15" t="s">
         <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
       </c>
       <c r="C17"/>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E17"/>
       <c r="F17"/>
-    </row>
-    <row r="18">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18"/>
-      <c r="F18"/>
-    </row>
-    <row r="19">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19"/>
-      <c r="F19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -837,10 +806,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -915,7 +884,7 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -932,10 +901,10 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
@@ -981,7 +950,7 @@
         <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8">
@@ -1076,7 +1045,7 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>40</v>
@@ -1092,7 +1061,7 @@
         <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
         <v>23</v>
@@ -1107,62 +1076,40 @@
       <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
+      <c r="C15"/>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16"/>
       <c r="F16"/>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
         <v>35</v>
       </c>
       <c r="C17"/>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E17"/>
       <c r="F17"/>
-    </row>
-    <row r="18">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18"/>
-      <c r="F18"/>
-    </row>
-    <row r="19">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19"/>
-      <c r="F19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>